<commit_message>
[WIP] Cambio de forma de PCB y componentes de Mouser
</commit_message>
<xml_diff>
--- a/GERBERS & BoM PCB_dHandlebar_Lateral/BoM - PCB_dHandlebar_Lateral.xlsx
+++ b/GERBERS & BoM PCB_dHandlebar_Lateral/BoM - PCB_dHandlebar_Lateral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[Proyectos]\Kit-CaminadorElectrico\PCB&amp;FW\Prototipo\dHandlebars\PCB_dHandlebar_Lateral\GERBERS &amp; BoM PCB_dHandlebar_Lateral\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D147572A-80E0-4CCB-8230-E0F7BDAF89AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100D612D-16DF-4FAF-8B22-7CB01E82510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -63,7 +63,7 @@
     <t>PCB_dHandlebar_Lateral.PrjPcb</t>
   </si>
   <si>
-    <t>15:18</t>
+    <t>12:11</t>
   </si>
   <si>
     <t>14</t>
@@ -117,10 +117,19 @@
     <t>Supplier 1</t>
   </si>
   <si>
-    <t>Farnell</t>
+    <t>Digi-Key</t>
   </si>
   <si>
     <t>Supplier Part Number 1</t>
+  </si>
+  <si>
+    <t>QLS6B-FKW-CNSNSF043CT-ND</t>
+  </si>
+  <si>
+    <t>P16063CT-ND</t>
+  </si>
+  <si>
+    <t>401-1910-1-ND</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -999,7 +1008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1095,7 +1106,7 @@
       </c>
       <c r="D7" s="13">
         <f ca="1">NOW()</f>
-        <v>45259.638015972225</v>
+        <v>45260.508200231481</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="53"/>
@@ -1123,7 +1134,7 @@
         <v>29</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
@@ -1144,8 +1155,8 @@
       <c r="F9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="37">
-        <v>3217314</v>
+      <c r="G9" s="37" t="s">
+        <v>30</v>
       </c>
       <c r="H9" s="40">
         <v>1</v>
@@ -1190,8 +1201,8 @@
       <c r="F11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="37">
-        <v>1750745</v>
+      <c r="G11" s="37" t="s">
+        <v>31</v>
       </c>
       <c r="H11" s="40">
         <v>3</v>
@@ -1215,8 +1226,8 @@
       <c r="F12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="37">
-        <v>3780578</v>
+      <c r="G12" s="37" t="s">
+        <v>32</v>
       </c>
       <c r="H12" s="40">
         <v>1</v>

</xml_diff>

<commit_message>
[WIP] Enrutado y ficheros de fabricacion de la LEFT
</commit_message>
<xml_diff>
--- a/GERBERS & BoM PCB_dHandlebar_Lateral/BoM - PCB_dHandlebar_Lateral.xlsx
+++ b/GERBERS & BoM PCB_dHandlebar_Lateral/BoM - PCB_dHandlebar_Lateral.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[Proyectos]\Kit-CaminadorElectrico\PCB&amp;FW\Prototipo\dHandlebars\PCB_dHandlebar_Lateral\GERBERS &amp; BoM PCB_dHandlebar_Lateral\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100D612D-16DF-4FAF-8B22-7CB01E82510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F287EAF5-B761-4E67-937A-B340D47503AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="4830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -57,16 +57,19 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Bill of Materials for Project [PCB_dHandlebar_Lateral.PrjPcb] (No PCB Document Selected)</t>
+    <t>Bill of Materials for PCB Document [PCB_dHandlebar_Lateral_Left.PcbDoc]</t>
+  </si>
+  <si>
+    <t>PCB_dHandlebar_Lateral_Left.PcbDoc</t>
   </si>
   <si>
     <t>PCB_dHandlebar_Lateral.PrjPcb</t>
   </si>
   <si>
-    <t>12:11</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>11:34</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>Designator</t>
@@ -75,9 +78,15 @@
     <t>D1</t>
   </si>
   <si>
+    <t>FD1, FD2, FD3</t>
+  </si>
+  <si>
     <t>P1, P2, P3, P4, P5, P6, P7, P8, P9</t>
   </si>
   <si>
+    <t>Pipe</t>
+  </si>
+  <si>
     <t>R1, R2, R3</t>
   </si>
   <si>
@@ -90,6 +99,9 @@
     <t>LED RGB QLS6B-FKW-CNSNSF043</t>
   </si>
   <si>
+    <t>FIDUCIAL</t>
+  </si>
+  <si>
     <t>CONNECTOR PAD</t>
   </si>
   <si>
@@ -105,6 +117,9 @@
     <t>LED, Superior, Transparente, RGB, Rojo, Verde, Azul, SMD, 120°, Redondo, R 30mA, V 30mA, B 30mA</t>
   </si>
   <si>
+    <t>Fiducial</t>
+  </si>
+  <si>
     <t>Conector Pad</t>
   </si>
   <si>
@@ -117,19 +132,19 @@
     <t>Supplier 1</t>
   </si>
   <si>
-    <t>Digi-Key</t>
+    <t>Mouser</t>
   </si>
   <si>
     <t>Supplier Part Number 1</t>
   </si>
   <si>
-    <t>QLS6B-FKW-CNSNSF043CT-ND</t>
-  </si>
-  <si>
-    <t>P16063CT-ND</t>
-  </si>
-  <si>
-    <t>401-1910-1-ND</t>
+    <t>941-QLS6BFKWNSNSF043</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F1800V</t>
+  </si>
+  <si>
+    <t>611-KSC541JROHS</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -619,18 +634,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -645,20 +648,32 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B9" sqref="B9:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,8 +1046,8 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
@@ -1040,11 +1055,11 @@
       <c r="C2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -1052,13 +1067,13 @@
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
@@ -1066,13 +1081,13 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="43" t="s">
-        <v>9</v>
+      <c r="D4" s="52" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="54"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -1080,9 +1095,9 @@
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
@@ -1090,13 +1105,13 @@
       <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="44" t="s">
-        <v>10</v>
+      <c r="D6" s="53" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
@@ -1106,12 +1121,12 @@
       </c>
       <c r="D7" s="13">
         <f ca="1">NOW()</f>
-        <v>45260.508200231481</v>
+        <v>45265.482350115744</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
@@ -1119,22 +1134,22 @@
         <v>4</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
@@ -1144,19 +1159,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H9" s="40">
         <v>1</v>
@@ -1169,131 +1184,169 @@
         <v>2</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="37"/>
       <c r="H10" s="40">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="39">
         <f>ROW(B11) - ROW($B$8)</f>
         <v>3</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="39">
         <f>ROW(B12) - ROW($B$8)</f>
         <v>4</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>32</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="40">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="39">
+        <f>ROW(B13) - ROW($B$8)</f>
         <v>5</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="39">
+        <f>ROW(B14) - ROW($B$8)</f>
+        <v>6</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="40">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="35"/>
+      <c r="B15" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="54" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="34"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="35"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="36"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="F3:H7"/>

</xml_diff>